<commit_message>
Change demand to week
</commit_message>
<xml_diff>
--- a/data/norway_demand.xlsx
+++ b/data/norway_demand.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MORFRE/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MORFRE/side_projects/hackaton-energy-game/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{342B24B8-DBD1-3A41-94ED-7AA890FE4DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA01172D-57F2-F44A-BAA2-FE2C54D1B2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{1170699B-E0F6-4D41-85E0-333D2367EE46}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="169">
   <si>
     <t>01.01.2024 00:00:00 +01:00</t>
   </si>
@@ -108,6 +108,441 @@
   </si>
   <si>
     <t>01.01.2024 23:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 00:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 01:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 02:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 03:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 04:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 05:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 06:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 07:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 08:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 09:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 10:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 11:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 12:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 13:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 14:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 15:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 16:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 17:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 18:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 19:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 20:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 21:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 22:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>02.01.2024 23:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 00:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 01:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 02:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 03:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 04:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 05:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 06:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 07:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 08:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 09:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 10:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 11:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 12:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 13:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 14:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 15:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 16:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 17:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 18:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 19:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 20:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 21:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 22:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>03.01.2024 23:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 00:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 01:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 02:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 03:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 04:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 05:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 06:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 07:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 08:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 09:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 10:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 11:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 12:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 13:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 14:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 15:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 16:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 17:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 18:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 19:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 20:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 21:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 22:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>04.01.2024 23:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 00:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 01:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 02:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 03:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 04:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 05:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 06:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 07:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 08:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 09:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 10:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 11:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 12:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 13:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 14:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 15:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 16:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 17:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 18:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 19:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 20:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 21:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 22:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>05.01.2024 23:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 00:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 01:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 02:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 03:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 04:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 05:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 06:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 07:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 08:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 09:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 10:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 11:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 12:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 13:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 14:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 15:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 16:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 17:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 18:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 19:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 20:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 21:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 22:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>06.01.2024 23:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 00:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 01:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 02:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 03:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 04:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 05:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 06:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 07:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 08:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 09:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 10:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 11:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 12:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 13:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 14:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 15:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 16:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 17:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 18:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 19:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 20:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 21:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 22:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>07.01.2024 23:00:00 +01:00</t>
+  </si>
+  <si>
+    <t>08.01.2024 00:00:00 +01:00</t>
   </si>
 </sst>
 </file>
@@ -483,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC90ECD-BDB8-8743-AFF5-D8DE7213C8B6}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C24"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="C192" sqref="A170:C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -755,6 +1190,1716 @@
         <v>19132</v>
       </c>
     </row>
+    <row r="25" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>13005</v>
+      </c>
+      <c r="C25" s="1">
+        <v>18836</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>12815</v>
+      </c>
+      <c r="C26" s="1">
+        <v>18755</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>12597</v>
+      </c>
+      <c r="C27" s="1">
+        <v>18523</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>12445</v>
+      </c>
+      <c r="C28" s="1">
+        <v>18527</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>12352</v>
+      </c>
+      <c r="C29" s="1">
+        <v>18655</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>13094</v>
+      </c>
+      <c r="C30" s="1">
+        <v>19037</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>14291</v>
+      </c>
+      <c r="C31" s="1">
+        <v>19996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
+        <v>16543</v>
+      </c>
+      <c r="C32" s="1">
+        <v>21245</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
+        <v>19230</v>
+      </c>
+      <c r="C33" s="1">
+        <v>22070</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1">
+        <v>20974</v>
+      </c>
+      <c r="C34" s="1">
+        <v>22374</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1">
+        <v>23153</v>
+      </c>
+      <c r="C35" s="1">
+        <v>22552</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1">
+        <v>24013</v>
+      </c>
+      <c r="C36" s="1">
+        <v>22789</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1">
+        <v>24864</v>
+      </c>
+      <c r="C37" s="1">
+        <v>22845</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1">
+        <v>24462</v>
+      </c>
+      <c r="C38" s="1">
+        <v>22418</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1">
+        <v>24505</v>
+      </c>
+      <c r="C39" s="1">
+        <v>22663</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1">
+        <v>25187</v>
+      </c>
+      <c r="C40" s="1">
+        <v>22934</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>25278</v>
+      </c>
+      <c r="C41" s="1">
+        <v>22974</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1">
+        <v>24884</v>
+      </c>
+      <c r="C42" s="1">
+        <v>22753</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1">
+        <v>22794</v>
+      </c>
+      <c r="C43" s="1">
+        <v>22541</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1">
+        <v>20105</v>
+      </c>
+      <c r="C44" s="1">
+        <v>22380</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1">
+        <v>18905</v>
+      </c>
+      <c r="C45" s="1">
+        <v>22291</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1">
+        <v>17717</v>
+      </c>
+      <c r="C46" s="1">
+        <v>21863</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1">
+        <v>16624</v>
+      </c>
+      <c r="C47" s="1">
+        <v>21433</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1">
+        <v>15786</v>
+      </c>
+      <c r="C48" s="1">
+        <v>20878</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1">
+        <v>15323</v>
+      </c>
+      <c r="C49" s="1">
+        <v>20508</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1">
+        <v>14985</v>
+      </c>
+      <c r="C50" s="1">
+        <v>20013</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1">
+        <v>15264</v>
+      </c>
+      <c r="C51" s="1">
+        <v>19786</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1">
+        <v>14713</v>
+      </c>
+      <c r="C52" s="1">
+        <v>19760</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1">
+        <v>14585</v>
+      </c>
+      <c r="C53" s="1">
+        <v>19768</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1">
+        <v>15379</v>
+      </c>
+      <c r="C54" s="1">
+        <v>20134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1">
+        <v>17067</v>
+      </c>
+      <c r="C55" s="1">
+        <v>21269</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1">
+        <v>19162</v>
+      </c>
+      <c r="C56" s="1">
+        <v>22617</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1">
+        <v>19886</v>
+      </c>
+      <c r="C57" s="1">
+        <v>22999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1">
+        <v>21020</v>
+      </c>
+      <c r="C58" s="1">
+        <v>23134</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1">
+        <v>21564</v>
+      </c>
+      <c r="C59" s="1">
+        <v>23201</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1">
+        <v>20823</v>
+      </c>
+      <c r="C60" s="1">
+        <v>23066</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1">
+        <v>20652</v>
+      </c>
+      <c r="C61" s="1">
+        <v>22987</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1">
+        <v>20722</v>
+      </c>
+      <c r="C62" s="1">
+        <v>23336</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1">
+        <v>21487</v>
+      </c>
+      <c r="C63" s="1">
+        <v>23360</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1">
+        <v>22952</v>
+      </c>
+      <c r="C64" s="1">
+        <v>23619</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1">
+        <v>24697</v>
+      </c>
+      <c r="C65" s="1">
+        <v>24070</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1">
+        <v>26037</v>
+      </c>
+      <c r="C66" s="1">
+        <v>23605</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1">
+        <v>26433</v>
+      </c>
+      <c r="C67" s="1">
+        <v>23204</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1">
+        <v>25481</v>
+      </c>
+      <c r="C68" s="1">
+        <v>22994</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1">
+        <v>23663</v>
+      </c>
+      <c r="C69" s="1">
+        <v>22838</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1">
+        <v>21687</v>
+      </c>
+      <c r="C70" s="1">
+        <v>22436</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1">
+        <v>19687</v>
+      </c>
+      <c r="C71" s="1">
+        <v>21978</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1">
+        <v>17449</v>
+      </c>
+      <c r="C72" s="1">
+        <v>21477</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1">
+        <v>16802</v>
+      </c>
+      <c r="C73" s="1">
+        <v>21066</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1">
+        <v>16359</v>
+      </c>
+      <c r="C74" s="1">
+        <v>20614</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1">
+        <v>16294</v>
+      </c>
+      <c r="C75" s="1">
+        <v>20343</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1">
+        <v>16349</v>
+      </c>
+      <c r="C76" s="1">
+        <v>20352</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1">
+        <v>16283</v>
+      </c>
+      <c r="C77" s="1">
+        <v>20358</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1">
+        <v>17012</v>
+      </c>
+      <c r="C78" s="1">
+        <v>20578</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1">
+        <v>21064</v>
+      </c>
+      <c r="C79" s="1">
+        <v>21876</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1">
+        <v>25606</v>
+      </c>
+      <c r="C80" s="1">
+        <v>23222</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1">
+        <v>26173</v>
+      </c>
+      <c r="C81" s="1">
+        <v>23427</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1">
+        <v>26068</v>
+      </c>
+      <c r="C82" s="1">
+        <v>23503</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1">
+        <v>26754</v>
+      </c>
+      <c r="C83" s="1">
+        <v>23476</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1">
+        <v>26270</v>
+      </c>
+      <c r="C84" s="1">
+        <v>23673</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1">
+        <v>26022</v>
+      </c>
+      <c r="C85" s="1">
+        <v>23502</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1">
+        <v>25950</v>
+      </c>
+      <c r="C86" s="1">
+        <v>23597</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1">
+        <v>27007</v>
+      </c>
+      <c r="C87" s="1">
+        <v>23766</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1">
+        <v>27175</v>
+      </c>
+      <c r="C88" s="1">
+        <v>24011</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1">
+        <v>27518</v>
+      </c>
+      <c r="C89" s="1">
+        <v>24506</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90" s="1">
+        <v>27379</v>
+      </c>
+      <c r="C90" s="1">
+        <v>24218</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1">
+        <v>27377</v>
+      </c>
+      <c r="C91" s="1">
+        <v>24094</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1">
+        <v>27410</v>
+      </c>
+      <c r="C92" s="1">
+        <v>24128</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1">
+        <v>27044</v>
+      </c>
+      <c r="C93" s="1">
+        <v>23754</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1">
+        <v>26307</v>
+      </c>
+      <c r="C94" s="1">
+        <v>23327</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B95" s="1">
+        <v>25692</v>
+      </c>
+      <c r="C95" s="1">
+        <v>22847</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1">
+        <v>25263</v>
+      </c>
+      <c r="C96" s="1">
+        <v>22203</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1">
+        <v>23698</v>
+      </c>
+      <c r="C97" s="1">
+        <v>21759</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1">
+        <v>22907</v>
+      </c>
+      <c r="C98" s="1">
+        <v>21386</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1">
+        <v>22276</v>
+      </c>
+      <c r="C99" s="1">
+        <v>21245</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1">
+        <v>21758</v>
+      </c>
+      <c r="C100" s="1">
+        <v>21277</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101" s="1">
+        <v>21849</v>
+      </c>
+      <c r="C101" s="1">
+        <v>21363</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B102" s="1">
+        <v>22325</v>
+      </c>
+      <c r="C102" s="1">
+        <v>21637</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B103" s="1">
+        <v>23566</v>
+      </c>
+      <c r="C103" s="1">
+        <v>22715</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B104" s="1">
+        <v>25268</v>
+      </c>
+      <c r="C104" s="1">
+        <v>24145</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B105" s="1">
+        <v>25433</v>
+      </c>
+      <c r="C105" s="1">
+        <v>24678</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B106" s="1">
+        <v>25758</v>
+      </c>
+      <c r="C106" s="1">
+        <v>24908</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B107" s="1">
+        <v>26015</v>
+      </c>
+      <c r="C107" s="1">
+        <v>24930</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B108" s="1">
+        <v>26029</v>
+      </c>
+      <c r="C108" s="1">
+        <v>24887</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B109" s="1">
+        <v>24938</v>
+      </c>
+      <c r="C109" s="1">
+        <v>24534</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B110" s="1">
+        <v>24650</v>
+      </c>
+      <c r="C110" s="1">
+        <v>24322</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B111" s="1">
+        <v>24719</v>
+      </c>
+      <c r="C111" s="1">
+        <v>24105</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B112" s="1">
+        <v>24571</v>
+      </c>
+      <c r="C112" s="1">
+        <v>24026</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B113" s="1">
+        <v>24353</v>
+      </c>
+      <c r="C113" s="1">
+        <v>24011</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B114" s="1">
+        <v>24260</v>
+      </c>
+      <c r="C114" s="1">
+        <v>23867</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B115" s="1">
+        <v>24078</v>
+      </c>
+      <c r="C115" s="1">
+        <v>23567</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B116" s="1">
+        <v>24605</v>
+      </c>
+      <c r="C116" s="1">
+        <v>23480</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B117" s="1">
+        <v>24690</v>
+      </c>
+      <c r="C117" s="1">
+        <v>23250</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B118" s="1">
+        <v>24856</v>
+      </c>
+      <c r="C118" s="1">
+        <v>22976</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B119" s="1">
+        <v>24595</v>
+      </c>
+      <c r="C119" s="1">
+        <v>22634</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B120" s="1">
+        <v>24030</v>
+      </c>
+      <c r="C120" s="1">
+        <v>22281</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B121" s="1">
+        <v>23293</v>
+      </c>
+      <c r="C121" s="1">
+        <v>21945</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B122" s="1">
+        <v>23019</v>
+      </c>
+      <c r="C122" s="1">
+        <v>21762</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B123" s="1">
+        <v>22534</v>
+      </c>
+      <c r="C123" s="1">
+        <v>21643</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B124" s="1">
+        <v>22128</v>
+      </c>
+      <c r="C124" s="1">
+        <v>21506</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B125" s="1">
+        <v>21803</v>
+      </c>
+      <c r="C125" s="1">
+        <v>21439</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B126" s="1">
+        <v>21463</v>
+      </c>
+      <c r="C126" s="1">
+        <v>21388</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B127" s="1">
+        <v>21646</v>
+      </c>
+      <c r="C127" s="1">
+        <v>21589</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B128" s="1">
+        <v>22295</v>
+      </c>
+      <c r="C128" s="1">
+        <v>21936</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B129" s="1">
+        <v>22634</v>
+      </c>
+      <c r="C129" s="1">
+        <v>22471</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B130" s="1">
+        <v>23320</v>
+      </c>
+      <c r="C130" s="1">
+        <v>22971</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B131" s="1">
+        <v>24225</v>
+      </c>
+      <c r="C131" s="1">
+        <v>23469</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B132" s="1">
+        <v>25058</v>
+      </c>
+      <c r="C132" s="1">
+        <v>23793</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B133" s="1">
+        <v>24897</v>
+      </c>
+      <c r="C133" s="1">
+        <v>23551</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B134" s="1">
+        <v>24552</v>
+      </c>
+      <c r="C134" s="1">
+        <v>23312</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B135" s="1">
+        <v>24282</v>
+      </c>
+      <c r="C135" s="1">
+        <v>23258</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B136" s="1">
+        <v>24616</v>
+      </c>
+      <c r="C136" s="1">
+        <v>23399</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B137" s="1">
+        <v>25360</v>
+      </c>
+      <c r="C137" s="1">
+        <v>23898</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B138" s="1">
+        <v>25864</v>
+      </c>
+      <c r="C138" s="1">
+        <v>24137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B139" s="1">
+        <v>25525</v>
+      </c>
+      <c r="C139" s="1">
+        <v>24130</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B140" s="1">
+        <v>24965</v>
+      </c>
+      <c r="C140" s="1">
+        <v>23786</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B141" s="1">
+        <v>24678</v>
+      </c>
+      <c r="C141" s="1">
+        <v>23281</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B142" s="1">
+        <v>23612</v>
+      </c>
+      <c r="C142" s="1">
+        <v>22723</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B143" s="1">
+        <v>22674</v>
+      </c>
+      <c r="C143" s="1">
+        <v>22488</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B144" s="1">
+        <v>22087</v>
+      </c>
+      <c r="C144" s="1">
+        <v>22007</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B145" s="1">
+        <v>23325</v>
+      </c>
+      <c r="C145" s="1">
+        <v>22060</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B146" s="1">
+        <v>23178</v>
+      </c>
+      <c r="C146" s="1">
+        <v>21746</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B147" s="1">
+        <v>22140</v>
+      </c>
+      <c r="C147" s="1">
+        <v>21576</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B148" s="1">
+        <v>21468</v>
+      </c>
+      <c r="C148" s="1">
+        <v>21452</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B149" s="1">
+        <v>21281</v>
+      </c>
+      <c r="C149" s="1">
+        <v>21514</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B150" s="1">
+        <v>21054</v>
+      </c>
+      <c r="C150" s="1">
+        <v>21466</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B151" s="1">
+        <v>21190</v>
+      </c>
+      <c r="C151" s="1">
+        <v>21547</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B152" s="1">
+        <v>21816</v>
+      </c>
+      <c r="C152" s="1">
+        <v>21770</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B153" s="1">
+        <v>22242</v>
+      </c>
+      <c r="C153" s="1">
+        <v>22188</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B154" s="1">
+        <v>23363</v>
+      </c>
+      <c r="C154" s="1">
+        <v>22748</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B155" s="1">
+        <v>24700</v>
+      </c>
+      <c r="C155" s="1">
+        <v>23169</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B156" s="1">
+        <v>24798</v>
+      </c>
+      <c r="C156" s="1">
+        <v>23120</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B157" s="1">
+        <v>24127</v>
+      </c>
+      <c r="C157" s="1">
+        <v>22966</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B158" s="1">
+        <v>23919</v>
+      </c>
+      <c r="C158" s="1">
+        <v>22938</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A159" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B159" s="1">
+        <v>23557</v>
+      </c>
+      <c r="C159" s="1">
+        <v>23066</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A160" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B160" s="1">
+        <v>23757</v>
+      </c>
+      <c r="C160" s="1">
+        <v>23320</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A161" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B161" s="1">
+        <v>23854</v>
+      </c>
+      <c r="C161" s="1">
+        <v>23628</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A162" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B162" s="1">
+        <v>24655</v>
+      </c>
+      <c r="C162" s="1">
+        <v>23726</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A163" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B163" s="1">
+        <v>24545</v>
+      </c>
+      <c r="C163" s="1">
+        <v>23497</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A164" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B164" s="1">
+        <v>24344</v>
+      </c>
+      <c r="C164" s="1">
+        <v>23301</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A165" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B165" s="1">
+        <v>24460</v>
+      </c>
+      <c r="C165" s="1">
+        <v>23077</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A166" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B166" s="1">
+        <v>24306</v>
+      </c>
+      <c r="C166" s="1">
+        <v>22843</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A167" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B167" s="1">
+        <v>24049</v>
+      </c>
+      <c r="C167" s="1">
+        <v>22555</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B168" s="1">
+        <v>22865</v>
+      </c>
+      <c r="C168" s="1">
+        <v>22037</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B169" s="1">
+        <v>22018</v>
+      </c>
+      <c r="C169" s="1">
+        <v>21582</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
+      <c r="C172" s="1"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
+      <c r="C173" s="1"/>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="1"/>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="1"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
+      <c r="C178" s="1"/>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
+      <c r="C179" s="1"/>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
+      <c r="C180" s="1"/>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="1"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" s="1"/>
+      <c r="B182" s="1"/>
+      <c r="C182" s="1"/>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" s="1"/>
+      <c r="B183" s="1"/>
+      <c r="C183" s="1"/>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" s="1"/>
+      <c r="B184" s="1"/>
+      <c r="C184" s="1"/>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" s="1"/>
+      <c r="B185" s="1"/>
+      <c r="C185" s="1"/>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" s="1"/>
+      <c r="B186" s="1"/>
+      <c r="C186" s="1"/>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" s="1"/>
+      <c r="B187" s="1"/>
+      <c r="C187" s="1"/>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" s="1"/>
+      <c r="B188" s="1"/>
+      <c r="C188" s="1"/>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" s="1"/>
+      <c r="B189" s="1"/>
+      <c r="C189" s="1"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" s="1"/>
+      <c r="B190" s="1"/>
+      <c r="C190" s="1"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" s="1"/>
+      <c r="B191" s="1"/>
+      <c r="C191" s="1"/>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" s="1"/>
+      <c r="B192" s="1"/>
+      <c r="C192" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>